<commit_message>
onboard flow - chronic
</commit_message>
<xml_diff>
--- a/dataFiles/onboarding/onboardingMH.xlsx
+++ b/dataFiles/onboarding/onboardingMH.xlsx
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
onboard flow - chronic (#13)
</commit_message>
<xml_diff>
--- a/dataFiles/onboarding/onboardingMH.xlsx
+++ b/dataFiles/onboarding/onboardingMH.xlsx
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mary/mind zone lessons (#15)
* MindZoneLessons_MentalHealth

* mind zone

* mental health lessons

---------

Co-authored-by: Immaculate1225 <mary.s@trackdfect.com>
</commit_message>
<xml_diff>
--- a/dataFiles/onboarding/onboardingMH.xlsx
+++ b/dataFiles/onboarding/onboardingMH.xlsx
@@ -495,7 +495,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>prabhapzqj7046@mailinator.com</t>
+    <t>prabhaAutohzLW5080@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>